<commit_message>
* fixed issue with displaying heal ratio in LiveReport * fixed issue with displaying group heal in Fight Report Window * added Entropy and Soul Trap ability detection for Scalebreaker
</commit_message>
<xml_diff>
--- a/SkillTimingData.xlsx
+++ b/SkillTimingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dk-mi\Documents\ESOdev\CombatMetrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A53C1A4-53D2-4362-9E51-588EB47C37A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9074F62D-2343-4A34-9F9B-30806ED2C208}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A7C7635A-D479-45C8-B72E-0189AC87FC44}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A7C7635A-D479-45C8-B72E-0189AC87FC44}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -383,6 +383,30 @@
   </si>
   <si>
     <t>Materialize</t>
+  </si>
+  <si>
+    <t>Mage Guild</t>
+  </si>
+  <si>
+    <t>Soul Trap</t>
+  </si>
+  <si>
+    <t>Entropy</t>
+  </si>
+  <si>
+    <t>Soul Magic</t>
+  </si>
+  <si>
+    <t>Degeneration</t>
+  </si>
+  <si>
+    <t>Soul Splitting Trap</t>
+  </si>
+  <si>
+    <t>Structured Entropy</t>
+  </si>
+  <si>
+    <t>Consuming Trap</t>
   </si>
 </sst>
 </file>
@@ -765,10 +789,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1306A4-11A6-4B75-940C-9ADFDFBE0CC7}">
-  <dimension ref="A1:G132"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2219,17 +2244,130 @@
         <v>1</v>
       </c>
     </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>119</v>
+      </c>
+      <c r="B136">
+        <v>28567</v>
+      </c>
+      <c r="C136">
+        <v>126370</v>
+      </c>
+      <c r="D136" t="s">
+        <v>119</v>
+      </c>
+      <c r="E136">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>121</v>
+      </c>
+      <c r="B137">
+        <v>40457</v>
+      </c>
+      <c r="C137">
+        <v>126374</v>
+      </c>
+      <c r="D137" t="s">
+        <v>121</v>
+      </c>
+      <c r="E137">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>123</v>
+      </c>
+      <c r="B138">
+        <v>40452</v>
+      </c>
+      <c r="C138">
+        <v>126371</v>
+      </c>
+      <c r="D138" t="s">
+        <v>123</v>
+      </c>
+      <c r="E138">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>118</v>
+      </c>
+      <c r="B142">
+        <v>26768</v>
+      </c>
+      <c r="C142">
+        <v>126891</v>
+      </c>
+      <c r="D142" t="s">
+        <v>118</v>
+      </c>
+      <c r="E142">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>122</v>
+      </c>
+      <c r="B143">
+        <v>40328</v>
+      </c>
+      <c r="C143">
+        <v>126894</v>
+      </c>
+      <c r="D143" t="s">
+        <v>122</v>
+      </c>
+      <c r="E143">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>124</v>
+      </c>
+      <c r="B144">
+        <v>40317</v>
+      </c>
+      <c r="C144">
+        <v>126896</v>
+      </c>
+      <c r="D144" t="s">
+        <v>124</v>
+      </c>
+      <c r="E144">
+        <v>2240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30D76D3A-1E84-4D87-A458-1F968EAA6EED}">
-  <dimension ref="A3:I134"/>
+  <dimension ref="A3:I147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H117" sqref="H117"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="I140" sqref="I140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6589,7 +6727,7 @@
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
         <f>IF(ISBLANK(Tabelle1!A134),"",Tabelle1!A134)</f>
-        <v/>
+        <v>Mage Guild</v>
       </c>
       <c r="B131" t="str">
         <f>IF(ISBLANK(Tabelle1!B134),"nil",Tabelle1!B134)</f>
@@ -6657,23 +6795,23 @@
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
         <f>IF(ISBLANK(Tabelle1!A136),"",Tabelle1!A136)</f>
-        <v/>
-      </c>
-      <c r="B133" t="str">
+        <v>Entropy</v>
+      </c>
+      <c r="B133">
         <f>IF(ISBLANK(Tabelle1!B136),"nil",Tabelle1!B136)</f>
-        <v>nil</v>
-      </c>
-      <c r="C133" t="str">
+        <v>28567</v>
+      </c>
+      <c r="C133">
         <f>IF(ISBLANK(Tabelle1!C136),"nil",Tabelle1!C136)</f>
-        <v>nil</v>
+        <v>126370</v>
       </c>
       <c r="D133" t="str">
         <f>IF(ISBLANK(Tabelle1!D136),"",Tabelle1!D136)</f>
-        <v/>
-      </c>
-      <c r="E133" t="str">
+        <v>Entropy</v>
+      </c>
+      <c r="E133">
         <f>IF(ISBLANK(Tabelle1!E136),"nil",Tabelle1!E136)</f>
-        <v>nil</v>
+        <v>2240</v>
       </c>
       <c r="F133" t="str">
         <f>IF(ISBLANK(Tabelle1!F136),"nil",Tabelle1!F136)</f>
@@ -6685,29 +6823,29 @@
       </c>
       <c r="I133" t="str">
         <f>IF(ISBLANK(Tabelle1!B136),"",CONCATENATE("[",B133,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C133,Tabelle2!E133:G133),"}, --", A133, " --&gt; ",D133))</f>
-        <v/>
+        <v>[28567] = {126370, 2240, nil, nil}, --Entropy --&gt; Entropy</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
         <f>IF(ISBLANK(Tabelle1!A137),"",Tabelle1!A137)</f>
-        <v/>
-      </c>
-      <c r="B134" t="str">
+        <v>Degeneration</v>
+      </c>
+      <c r="B134">
         <f>IF(ISBLANK(Tabelle1!B137),"nil",Tabelle1!B137)</f>
-        <v>nil</v>
-      </c>
-      <c r="C134" t="str">
+        <v>40457</v>
+      </c>
+      <c r="C134">
         <f>IF(ISBLANK(Tabelle1!C137),"nil",Tabelle1!C137)</f>
-        <v>nil</v>
+        <v>126374</v>
       </c>
       <c r="D134" t="str">
         <f>IF(ISBLANK(Tabelle1!D137),"",Tabelle1!D137)</f>
-        <v/>
-      </c>
-      <c r="E134" t="str">
+        <v>Degeneration</v>
+      </c>
+      <c r="E134">
         <f>IF(ISBLANK(Tabelle1!E137),"nil",Tabelle1!E137)</f>
-        <v>nil</v>
+        <v>2240</v>
       </c>
       <c r="F134" t="str">
         <f>IF(ISBLANK(Tabelle1!F137),"nil",Tabelle1!F137)</f>
@@ -6719,6 +6857,448 @@
       </c>
       <c r="I134" t="str">
         <f>IF(ISBLANK(Tabelle1!B137),"",CONCATENATE("[",B134,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C134,Tabelle2!E134:G134),"}, --", A134, " --&gt; ",D134))</f>
+        <v>[40457] = {126374, 2240, nil, nil}, --Degeneration --&gt; Degeneration</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="str">
+        <f>IF(ISBLANK(Tabelle1!A138),"",Tabelle1!A138)</f>
+        <v>Structured Entropy</v>
+      </c>
+      <c r="B135">
+        <f>IF(ISBLANK(Tabelle1!B138),"nil",Tabelle1!B138)</f>
+        <v>40452</v>
+      </c>
+      <c r="C135">
+        <f>IF(ISBLANK(Tabelle1!C138),"nil",Tabelle1!C138)</f>
+        <v>126371</v>
+      </c>
+      <c r="D135" t="str">
+        <f>IF(ISBLANK(Tabelle1!D138),"",Tabelle1!D138)</f>
+        <v>Structured Entropy</v>
+      </c>
+      <c r="E135">
+        <f>IF(ISBLANK(Tabelle1!E138),"nil",Tabelle1!E138)</f>
+        <v>2240</v>
+      </c>
+      <c r="F135" t="str">
+        <f>IF(ISBLANK(Tabelle1!F138),"nil",Tabelle1!F138)</f>
+        <v>nil</v>
+      </c>
+      <c r="G135" t="str">
+        <f>IF(ISBLANK(Tabelle1!G138),"nil",Tabelle1!G138)</f>
+        <v>nil</v>
+      </c>
+      <c r="I135" t="str">
+        <f>IF(ISBLANK(Tabelle1!B138),"",CONCATENATE("[",B135,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C135,Tabelle2!E135:G135),"}, --", A135, " --&gt; ",D135))</f>
+        <v>[40452] = {126371, 2240, nil, nil}, --Structured Entropy --&gt; Structured Entropy</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" t="str">
+        <f>IF(ISBLANK(Tabelle1!A139),"",Tabelle1!A139)</f>
+        <v/>
+      </c>
+      <c r="B136" t="str">
+        <f>IF(ISBLANK(Tabelle1!B139),"nil",Tabelle1!B139)</f>
+        <v>nil</v>
+      </c>
+      <c r="C136" t="str">
+        <f>IF(ISBLANK(Tabelle1!C139),"nil",Tabelle1!C139)</f>
+        <v>nil</v>
+      </c>
+      <c r="D136" t="str">
+        <f>IF(ISBLANK(Tabelle1!D139),"",Tabelle1!D139)</f>
+        <v/>
+      </c>
+      <c r="E136" t="str">
+        <f>IF(ISBLANK(Tabelle1!E139),"nil",Tabelle1!E139)</f>
+        <v>nil</v>
+      </c>
+      <c r="F136" t="str">
+        <f>IF(ISBLANK(Tabelle1!F139),"nil",Tabelle1!F139)</f>
+        <v>nil</v>
+      </c>
+      <c r="G136" t="str">
+        <f>IF(ISBLANK(Tabelle1!G139),"nil",Tabelle1!G139)</f>
+        <v>nil</v>
+      </c>
+      <c r="I136" t="str">
+        <f>IF(ISBLANK(Tabelle1!B139),"",CONCATENATE("[",B136,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C136,Tabelle2!E136:G136),"}, --", A136, " --&gt; ",D136))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" t="str">
+        <f>IF(ISBLANK(Tabelle1!A140),"",Tabelle1!A140)</f>
+        <v>Soul Magic</v>
+      </c>
+      <c r="B137" t="str">
+        <f>IF(ISBLANK(Tabelle1!B140),"nil",Tabelle1!B140)</f>
+        <v>nil</v>
+      </c>
+      <c r="C137" t="str">
+        <f>IF(ISBLANK(Tabelle1!C140),"nil",Tabelle1!C140)</f>
+        <v>nil</v>
+      </c>
+      <c r="D137" t="str">
+        <f>IF(ISBLANK(Tabelle1!D140),"",Tabelle1!D140)</f>
+        <v/>
+      </c>
+      <c r="E137" t="str">
+        <f>IF(ISBLANK(Tabelle1!E140),"nil",Tabelle1!E140)</f>
+        <v>nil</v>
+      </c>
+      <c r="F137" t="str">
+        <f>IF(ISBLANK(Tabelle1!F140),"nil",Tabelle1!F140)</f>
+        <v>nil</v>
+      </c>
+      <c r="G137" t="str">
+        <f>IF(ISBLANK(Tabelle1!G140),"nil",Tabelle1!G140)</f>
+        <v>nil</v>
+      </c>
+      <c r="I137" t="str">
+        <f>IF(ISBLANK(Tabelle1!B140),"",CONCATENATE("[",B137,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C137,Tabelle2!E137:G137),"}, --", A137, " --&gt; ",D137))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="str">
+        <f>IF(ISBLANK(Tabelle1!A141),"",Tabelle1!A141)</f>
+        <v/>
+      </c>
+      <c r="B138" t="str">
+        <f>IF(ISBLANK(Tabelle1!B141),"nil",Tabelle1!B141)</f>
+        <v>nil</v>
+      </c>
+      <c r="C138" t="str">
+        <f>IF(ISBLANK(Tabelle1!C141),"nil",Tabelle1!C141)</f>
+        <v>nil</v>
+      </c>
+      <c r="D138" t="str">
+        <f>IF(ISBLANK(Tabelle1!D141),"",Tabelle1!D141)</f>
+        <v/>
+      </c>
+      <c r="E138" t="str">
+        <f>IF(ISBLANK(Tabelle1!E141),"nil",Tabelle1!E141)</f>
+        <v>nil</v>
+      </c>
+      <c r="F138" t="str">
+        <f>IF(ISBLANK(Tabelle1!F141),"nil",Tabelle1!F141)</f>
+        <v>nil</v>
+      </c>
+      <c r="G138" t="str">
+        <f>IF(ISBLANK(Tabelle1!G141),"nil",Tabelle1!G141)</f>
+        <v>nil</v>
+      </c>
+      <c r="I138" t="str">
+        <f>IF(ISBLANK(Tabelle1!B141),"",CONCATENATE("[",B138,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C138,Tabelle2!E138:G138),"}, --", A138, " --&gt; ",D138))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" t="str">
+        <f>IF(ISBLANK(Tabelle1!A142),"",Tabelle1!A142)</f>
+        <v>Soul Trap</v>
+      </c>
+      <c r="B139">
+        <f>IF(ISBLANK(Tabelle1!B142),"nil",Tabelle1!B142)</f>
+        <v>26768</v>
+      </c>
+      <c r="C139">
+        <f>IF(ISBLANK(Tabelle1!C142),"nil",Tabelle1!C142)</f>
+        <v>126891</v>
+      </c>
+      <c r="D139" t="str">
+        <f>IF(ISBLANK(Tabelle1!D142),"",Tabelle1!D142)</f>
+        <v>Soul Trap</v>
+      </c>
+      <c r="E139">
+        <f>IF(ISBLANK(Tabelle1!E142),"nil",Tabelle1!E142)</f>
+        <v>2240</v>
+      </c>
+      <c r="F139" t="str">
+        <f>IF(ISBLANK(Tabelle1!F142),"nil",Tabelle1!F142)</f>
+        <v>nil</v>
+      </c>
+      <c r="G139" t="str">
+        <f>IF(ISBLANK(Tabelle1!G142),"nil",Tabelle1!G142)</f>
+        <v>nil</v>
+      </c>
+      <c r="I139" t="str">
+        <f>IF(ISBLANK(Tabelle1!B142),"",CONCATENATE("[",B139,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C139,Tabelle2!E139:G139),"}, --", A139, " --&gt; ",D139))</f>
+        <v>[26768] = {126891, 2240, nil, nil}, --Soul Trap --&gt; Soul Trap</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" t="str">
+        <f>IF(ISBLANK(Tabelle1!A143),"",Tabelle1!A143)</f>
+        <v>Soul Splitting Trap</v>
+      </c>
+      <c r="B140">
+        <f>IF(ISBLANK(Tabelle1!B143),"nil",Tabelle1!B143)</f>
+        <v>40328</v>
+      </c>
+      <c r="C140">
+        <f>IF(ISBLANK(Tabelle1!C143),"nil",Tabelle1!C143)</f>
+        <v>126894</v>
+      </c>
+      <c r="D140" t="str">
+        <f>IF(ISBLANK(Tabelle1!D143),"",Tabelle1!D143)</f>
+        <v>Soul Splitting Trap</v>
+      </c>
+      <c r="E140">
+        <f>IF(ISBLANK(Tabelle1!E143),"nil",Tabelle1!E143)</f>
+        <v>2240</v>
+      </c>
+      <c r="F140" t="str">
+        <f>IF(ISBLANK(Tabelle1!F143),"nil",Tabelle1!F143)</f>
+        <v>nil</v>
+      </c>
+      <c r="G140" t="str">
+        <f>IF(ISBLANK(Tabelle1!G143),"nil",Tabelle1!G143)</f>
+        <v>nil</v>
+      </c>
+      <c r="I140" t="str">
+        <f>IF(ISBLANK(Tabelle1!B143),"",CONCATENATE("[",B140,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C140,Tabelle2!E140:G140),"}, --", A140, " --&gt; ",D140))</f>
+        <v>[40328] = {126894, 2240, nil, nil}, --Soul Splitting Trap --&gt; Soul Splitting Trap</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" t="str">
+        <f>IF(ISBLANK(Tabelle1!A144),"",Tabelle1!A144)</f>
+        <v>Consuming Trap</v>
+      </c>
+      <c r="B141">
+        <f>IF(ISBLANK(Tabelle1!B144),"nil",Tabelle1!B144)</f>
+        <v>40317</v>
+      </c>
+      <c r="C141">
+        <f>IF(ISBLANK(Tabelle1!C144),"nil",Tabelle1!C144)</f>
+        <v>126896</v>
+      </c>
+      <c r="D141" t="str">
+        <f>IF(ISBLANK(Tabelle1!D144),"",Tabelle1!D144)</f>
+        <v>Consuming Trap</v>
+      </c>
+      <c r="E141">
+        <f>IF(ISBLANK(Tabelle1!E144),"nil",Tabelle1!E144)</f>
+        <v>2240</v>
+      </c>
+      <c r="F141" t="str">
+        <f>IF(ISBLANK(Tabelle1!F144),"nil",Tabelle1!F144)</f>
+        <v>nil</v>
+      </c>
+      <c r="G141" t="str">
+        <f>IF(ISBLANK(Tabelle1!G144),"nil",Tabelle1!G144)</f>
+        <v>nil</v>
+      </c>
+      <c r="I141" t="str">
+        <f>IF(ISBLANK(Tabelle1!B144),"",CONCATENATE("[",B141,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C141,Tabelle2!E141:G141),"}, --", A141, " --&gt; ",D141))</f>
+        <v>[40317] = {126896, 2240, nil, nil}, --Consuming Trap --&gt; Consuming Trap</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" t="str">
+        <f>IF(ISBLANK(Tabelle1!A145),"",Tabelle1!A145)</f>
+        <v/>
+      </c>
+      <c r="B142" t="str">
+        <f>IF(ISBLANK(Tabelle1!B145),"nil",Tabelle1!B145)</f>
+        <v>nil</v>
+      </c>
+      <c r="C142" t="str">
+        <f>IF(ISBLANK(Tabelle1!C145),"nil",Tabelle1!C145)</f>
+        <v>nil</v>
+      </c>
+      <c r="D142" t="str">
+        <f>IF(ISBLANK(Tabelle1!D145),"",Tabelle1!D145)</f>
+        <v/>
+      </c>
+      <c r="E142" t="str">
+        <f>IF(ISBLANK(Tabelle1!E145),"nil",Tabelle1!E145)</f>
+        <v>nil</v>
+      </c>
+      <c r="F142" t="str">
+        <f>IF(ISBLANK(Tabelle1!F145),"nil",Tabelle1!F145)</f>
+        <v>nil</v>
+      </c>
+      <c r="G142" t="str">
+        <f>IF(ISBLANK(Tabelle1!G145),"nil",Tabelle1!G145)</f>
+        <v>nil</v>
+      </c>
+      <c r="I142" t="str">
+        <f>IF(ISBLANK(Tabelle1!B145),"",CONCATENATE("[",B142,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C142,Tabelle2!E142:G142),"}, --", A142, " --&gt; ",D142))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="str">
+        <f>IF(ISBLANK(Tabelle1!A146),"",Tabelle1!A146)</f>
+        <v/>
+      </c>
+      <c r="B143" t="str">
+        <f>IF(ISBLANK(Tabelle1!B146),"nil",Tabelle1!B146)</f>
+        <v>nil</v>
+      </c>
+      <c r="C143" t="str">
+        <f>IF(ISBLANK(Tabelle1!C146),"nil",Tabelle1!C146)</f>
+        <v>nil</v>
+      </c>
+      <c r="D143" t="str">
+        <f>IF(ISBLANK(Tabelle1!D146),"",Tabelle1!D146)</f>
+        <v/>
+      </c>
+      <c r="E143" t="str">
+        <f>IF(ISBLANK(Tabelle1!E146),"nil",Tabelle1!E146)</f>
+        <v>nil</v>
+      </c>
+      <c r="F143" t="str">
+        <f>IF(ISBLANK(Tabelle1!F146),"nil",Tabelle1!F146)</f>
+        <v>nil</v>
+      </c>
+      <c r="G143" t="str">
+        <f>IF(ISBLANK(Tabelle1!G146),"nil",Tabelle1!G146)</f>
+        <v>nil</v>
+      </c>
+      <c r="I143" t="str">
+        <f>IF(ISBLANK(Tabelle1!B146),"",CONCATENATE("[",B143,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C143,Tabelle2!E143:G143),"}, --", A143, " --&gt; ",D143))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" t="str">
+        <f>IF(ISBLANK(Tabelle1!A147),"",Tabelle1!A147)</f>
+        <v/>
+      </c>
+      <c r="B144" t="str">
+        <f>IF(ISBLANK(Tabelle1!B147),"nil",Tabelle1!B147)</f>
+        <v>nil</v>
+      </c>
+      <c r="C144" t="str">
+        <f>IF(ISBLANK(Tabelle1!C147),"nil",Tabelle1!C147)</f>
+        <v>nil</v>
+      </c>
+      <c r="D144" t="str">
+        <f>IF(ISBLANK(Tabelle1!D147),"",Tabelle1!D147)</f>
+        <v/>
+      </c>
+      <c r="E144" t="str">
+        <f>IF(ISBLANK(Tabelle1!E147),"nil",Tabelle1!E147)</f>
+        <v>nil</v>
+      </c>
+      <c r="F144" t="str">
+        <f>IF(ISBLANK(Tabelle1!F147),"nil",Tabelle1!F147)</f>
+        <v>nil</v>
+      </c>
+      <c r="G144" t="str">
+        <f>IF(ISBLANK(Tabelle1!G147),"nil",Tabelle1!G147)</f>
+        <v>nil</v>
+      </c>
+      <c r="I144" t="str">
+        <f>IF(ISBLANK(Tabelle1!B147),"",CONCATENATE("[",B144,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C144,Tabelle2!E144:G144),"}, --", A144, " --&gt; ",D144))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" t="str">
+        <f>IF(ISBLANK(Tabelle1!A148),"",Tabelle1!A148)</f>
+        <v/>
+      </c>
+      <c r="B145" t="str">
+        <f>IF(ISBLANK(Tabelle1!B148),"nil",Tabelle1!B148)</f>
+        <v>nil</v>
+      </c>
+      <c r="C145" t="str">
+        <f>IF(ISBLANK(Tabelle1!C148),"nil",Tabelle1!C148)</f>
+        <v>nil</v>
+      </c>
+      <c r="D145" t="str">
+        <f>IF(ISBLANK(Tabelle1!D148),"",Tabelle1!D148)</f>
+        <v/>
+      </c>
+      <c r="E145" t="str">
+        <f>IF(ISBLANK(Tabelle1!E148),"nil",Tabelle1!E148)</f>
+        <v>nil</v>
+      </c>
+      <c r="F145" t="str">
+        <f>IF(ISBLANK(Tabelle1!F148),"nil",Tabelle1!F148)</f>
+        <v>nil</v>
+      </c>
+      <c r="G145" t="str">
+        <f>IF(ISBLANK(Tabelle1!G148),"nil",Tabelle1!G148)</f>
+        <v>nil</v>
+      </c>
+      <c r="I145" t="str">
+        <f>IF(ISBLANK(Tabelle1!B148),"",CONCATENATE("[",B145,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C145,Tabelle2!E145:G145),"}, --", A145, " --&gt; ",D145))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" t="str">
+        <f>IF(ISBLANK(Tabelle1!A149),"",Tabelle1!A149)</f>
+        <v/>
+      </c>
+      <c r="B146" t="str">
+        <f>IF(ISBLANK(Tabelle1!B149),"nil",Tabelle1!B149)</f>
+        <v>nil</v>
+      </c>
+      <c r="C146" t="str">
+        <f>IF(ISBLANK(Tabelle1!C149),"nil",Tabelle1!C149)</f>
+        <v>nil</v>
+      </c>
+      <c r="D146" t="str">
+        <f>IF(ISBLANK(Tabelle1!D149),"",Tabelle1!D149)</f>
+        <v/>
+      </c>
+      <c r="E146" t="str">
+        <f>IF(ISBLANK(Tabelle1!E149),"nil",Tabelle1!E149)</f>
+        <v>nil</v>
+      </c>
+      <c r="F146" t="str">
+        <f>IF(ISBLANK(Tabelle1!F149),"nil",Tabelle1!F149)</f>
+        <v>nil</v>
+      </c>
+      <c r="G146" t="str">
+        <f>IF(ISBLANK(Tabelle1!G149),"nil",Tabelle1!G149)</f>
+        <v>nil</v>
+      </c>
+      <c r="I146" t="str">
+        <f>IF(ISBLANK(Tabelle1!B149),"",CONCATENATE("[",B146,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C146,Tabelle2!E146:G146),"}, --", A146, " --&gt; ",D146))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" t="str">
+        <f>IF(ISBLANK(Tabelle1!A150),"",Tabelle1!A150)</f>
+        <v/>
+      </c>
+      <c r="B147" t="str">
+        <f>IF(ISBLANK(Tabelle1!B150),"nil",Tabelle1!B150)</f>
+        <v>nil</v>
+      </c>
+      <c r="C147" t="str">
+        <f>IF(ISBLANK(Tabelle1!C150),"nil",Tabelle1!C150)</f>
+        <v>nil</v>
+      </c>
+      <c r="D147" t="str">
+        <f>IF(ISBLANK(Tabelle1!D150),"",Tabelle1!D150)</f>
+        <v/>
+      </c>
+      <c r="E147" t="str">
+        <f>IF(ISBLANK(Tabelle1!E150),"nil",Tabelle1!E150)</f>
+        <v>nil</v>
+      </c>
+      <c r="F147" t="str">
+        <f>IF(ISBLANK(Tabelle1!F150),"nil",Tabelle1!F150)</f>
+        <v>nil</v>
+      </c>
+      <c r="G147" t="str">
+        <f>IF(ISBLANK(Tabelle1!G150),"nil",Tabelle1!G150)</f>
+        <v>nil</v>
+      </c>
+      <c r="I147" t="str">
+        <f>IF(ISBLANK(Tabelle1!B150),"",CONCATENATE("[",B147,"] = {",_xlfn.TEXTJOIN(", ", FALSE, Tabelle2!C147,Tabelle2!E147:G147),"}, --", A147, " --&gt; ",D147))</f>
         <v/>
       </c>
     </row>

</xml_diff>